<commit_message>
clean up of everything
</commit_message>
<xml_diff>
--- a/PHX2/part4/output2.xlsx
+++ b/PHX2/part4/output2.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,7 +442,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>WAR/pos</t>
         </is>
       </c>
     </row>
@@ -455,6 +460,9 @@
           <t>Ichiro Suzuki\suzukic01</t>
         </is>
       </c>
+      <c r="C2" t="n">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -465,6 +473,9 @@
           <t>Adrian Beltre\beltrad01</t>
         </is>
       </c>
+      <c r="C3" t="n">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -475,6 +486,9 @@
           <t>Franklin Gutierrez\gutiefr01</t>
         </is>
       </c>
+      <c r="C4" t="n">
+        <v>6.6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -485,6 +499,9 @@
           <t>Ichiro Suzuki\suzukic01</t>
         </is>
       </c>
+      <c r="C5" t="n">
+        <v>3.7</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -495,6 +512,9 @@
           <t>Brendan Ryan\ryanbr01</t>
         </is>
       </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -505,6 +525,9 @@
           <t>John Jaso\jasojo01</t>
         </is>
       </c>
+      <c r="C7" t="n">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -515,6 +538,9 @@
           <t>Kyle Seager\seageky01</t>
         </is>
       </c>
+      <c r="C8" t="n">
+        <v>3.9</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -525,6 +551,9 @@
           <t>Robinson Cano\canoro01</t>
         </is>
       </c>
+      <c r="C9" t="n">
+        <v>6.4</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -535,6 +564,9 @@
           <t>Nelson Cruz\cruzne02</t>
         </is>
       </c>
+      <c r="C10" t="n">
+        <v>5.2</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -544,6 +576,9 @@
         <is>
           <t>Robinson Cano\canoro01</t>
         </is>
+      </c>
+      <c r="C11" t="n">
+        <v>7.3</v>
       </c>
     </row>
   </sheetData>
@@ -557,7 +592,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -581,6 +616,16 @@
           <t>Year</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>OPS</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -594,6 +639,12 @@
       <c r="C2" t="n">
         <v>2015</v>
       </c>
+      <c r="D2" t="n">
+        <v>0.9360000000000001</v>
+      </c>
+      <c r="E2" t="n">
+        <v>590</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -607,6 +658,12 @@
       <c r="C3" t="n">
         <v>2016</v>
       </c>
+      <c r="D3" t="n">
+        <v>0.915</v>
+      </c>
+      <c r="E3" t="n">
+        <v>589</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -620,6 +677,12 @@
       <c r="C4" t="n">
         <v>2016</v>
       </c>
+      <c r="D4" t="n">
+        <v>0.882</v>
+      </c>
+      <c r="E4" t="n">
+        <v>655</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -633,6 +696,12 @@
       <c r="C5" t="n">
         <v>2009</v>
       </c>
+      <c r="D5" t="n">
+        <v>0.867</v>
+      </c>
+      <c r="E5" t="n">
+        <v>431</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -646,6 +715,12 @@
       <c r="C6" t="n">
         <v>2016</v>
       </c>
+      <c r="D6" t="n">
+        <v>0.859</v>
+      </c>
+      <c r="E6" t="n">
+        <v>597</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -659,6 +734,12 @@
       <c r="C7" t="n">
         <v>2009</v>
       </c>
+      <c r="D7" t="n">
+        <v>0.851</v>
+      </c>
+      <c r="E7" t="n">
+        <v>639</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -672,6 +753,12 @@
       <c r="C8" t="n">
         <v>2008</v>
       </c>
+      <c r="D8" t="n">
+        <v>0.837</v>
+      </c>
+      <c r="E8" t="n">
+        <v>635</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -685,6 +772,12 @@
       <c r="C9" t="n">
         <v>2014</v>
       </c>
+      <c r="D9" t="n">
+        <v>0.836</v>
+      </c>
+      <c r="E9" t="n">
+        <v>595</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -698,6 +791,12 @@
       <c r="C10" t="n">
         <v>2007</v>
       </c>
+      <c r="D10" t="n">
+        <v>0.831</v>
+      </c>
+      <c r="E10" t="n">
+        <v>573</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -710,6 +809,12 @@
       </c>
       <c r="C11" t="n">
         <v>2007</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.827</v>
+      </c>
+      <c r="E11" t="n">
+        <v>678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>